<commit_message>
feat: add funcionally disable checkbox on Configuration
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPathPrograms\Dispatcher_ContabilidadFacturas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E16AF2-DF3E-4059-BC72-E40B7B6A4432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2719AE7C-A7EE-4ABF-B893-09297ABA4654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16905" yWindow="1950" windowWidth="16860" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="2550" windowWidth="19770" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
     <t>Client_Email</t>
   </si>
   <si>
-    <t>antojse989@gmail.com</t>
+    <t>sarashattra@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -603,7 +603,7 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
fix: config_navegator and login
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPathPrograms\Dispatcher_ContabilidadFacturas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2719AE7C-A7EE-4ABF-B893-09297ABA4654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B3C754-B4B4-48CF-B770-ED2486F900DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="2550" windowWidth="19770" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>PathExceptionsFile</t>
   </si>
   <si>
-    <t>Data\\Exceptions.xlsx</t>
-  </si>
-  <si>
     <t>BECode_Credential</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   </si>
   <si>
     <t>sarashattra@gmail.com</t>
+  </si>
+  <si>
+    <t>C:\Exceptions.xlsx</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,7 +285,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,7 +602,7 @@
   <dimension ref="A1:Z19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -748,34 +747,34 @@
         <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" t="s">
         <v>64</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="C16" s="2"/>
     </row>

</xml_diff>

<commit_message>
feat: add check verification exist folders
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPathPrograms\Dispatcher_ContabilidadFacturas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B3C754-B4B4-48CF-B770-ED2486F900DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC484C70-F6B7-4B6B-BFB3-22F1F25F2463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -224,6 +224,12 @@
   </si>
   <si>
     <t>C:\Exceptions.xlsx</t>
+  </si>
+  <si>
+    <t>SE#007</t>
+  </si>
+  <si>
+    <t>SECode_Conection</t>
   </si>
 </sst>
 </file>
@@ -303,7 +309,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -599,13 +605,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z19"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -771,16 +777,20 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3">
@@ -792,6 +802,11 @@
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -808,7 +823,7 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -999,7 +1014,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>

</xml_diff>